<commit_message>
testrun completed and folder created for fullrun
</commit_message>
<xml_diff>
--- a/Threagile_testrun/risks.xlsx
+++ b/Threagile_testrun/risks.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Wahlpflichtmodul" sheetId="2" r:id="rId4"/>
+    <sheet name="Insecure IT Testmodell" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t>Severity</t>
   </si>
@@ -76,7 +76,7 @@
     <t>Ticket</t>
   </si>
   <si>
-    <t>Critical</t>
+    <t>Elevated</t>
   </si>
   <si>
     <t>Likely</t>
@@ -85,187 +85,238 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Repudiation</t>
+    <t>Tampering</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>CWE-79</t>
+  </si>
+  <si>
+    <t>Cross-Site Scripting (XSS)</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Cross-Site Scripting (XSS) risk at app</t>
+  </si>
+  <si>
+    <t>XSS Prevention</t>
+  </si>
+  <si>
+    <t>Try to encode all values sent back to the browser and also handle DOM-manipulations in a safe way to avoid DOM-based XSS. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>Are recommendations from the linked cheat sheet and referenced ASVS chapter applied?</t>
+  </si>
+  <si>
+    <t>cross-site-scripting@app</t>
+  </si>
+  <si>
+    <t>Unchecked</t>
+  </si>
+  <si>
+    <t>webapp</t>
+  </si>
+  <si>
+    <t>Cross-Site Scripting (XSS) risk at webapp</t>
+  </si>
+  <si>
+    <t>cross-site-scripting@webapp</t>
+  </si>
+  <si>
+    <t>Elevation of Privilege</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>CWE-306</t>
+  </si>
+  <si>
+    <t>Missing Authentication</t>
+  </si>
+  <si>
+    <t>to-app</t>
+  </si>
+  <si>
+    <t>Missing Authentication covering communication link to-app from webapp to app</t>
+  </si>
+  <si>
+    <t>Authentication of Incoming Requests</t>
+  </si>
+  <si>
+    <t>Apply an authentication method to the technical asset. To protect highly sensitive data consider the use of two-factor authentication for human users.</t>
+  </si>
+  <si>
+    <t>missing-authentication@webapp&gt;to-app@webapp@app</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>to-database</t>
+  </si>
+  <si>
+    <t>Missing Authentication covering communication link to-database from app to database</t>
+  </si>
+  <si>
+    <t>missing-authentication@app&gt;to-database@app@database</t>
+  </si>
+  <si>
+    <t>to-webapp</t>
+  </si>
+  <si>
+    <t>Missing Authentication covering communication link to-webapp from client to webapp</t>
+  </si>
+  <si>
+    <t>missing-authentication@client&gt;to-webapp@client@webapp</t>
+  </si>
+  <si>
+    <t>Very Likely</t>
+  </si>
+  <si>
+    <t>CWE-89</t>
+  </si>
+  <si>
+    <t>SQL/NoSQL-Injection</t>
+  </si>
+  <si>
+    <t>SQL/NoSQL-Injection risk at app against database database via to-database</t>
+  </si>
+  <si>
+    <t>SQL/NoSQL-Injection Prevention</t>
+  </si>
+  <si>
+    <t>Try to use parameter binding to be safe from injection vulnerabilities. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>sql-nosql-injection@app@database@app&gt;to-database</t>
+  </si>
+  <si>
+    <t>Information Disclosure</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>CWE-319</t>
+  </si>
+  <si>
+    <t>Unencrypted Communication</t>
+  </si>
+  <si>
+    <t>Unencrypted Communication named to-app between webapp and app</t>
+  </si>
+  <si>
+    <t>Encryption of Communication Links</t>
+  </si>
+  <si>
+    <t>Apply transport layer encryption to the communication link.</t>
+  </si>
+  <si>
+    <t>unencrypted-communication@webapp&gt;to-app@webapp@app</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>Unencrypted Communication named to-webapp between client and webapp</t>
+  </si>
+  <si>
+    <t>unencrypted-communication@client&gt;to-webapp@client@webapp</t>
+  </si>
+  <si>
+    <t>Unlikely</t>
+  </si>
+  <si>
+    <t>Unencrypted Communication named to-database between app and database</t>
+  </si>
+  <si>
+    <t>unencrypted-communication@app&gt;to-database@app@database</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Spoofing</t>
+  </si>
+  <si>
+    <t>CWE-352</t>
+  </si>
+  <si>
+    <t>Cross-Site Request Forgery (CSRF)</t>
+  </si>
+  <si>
+    <t>Cross-Site Request Forgery (CSRF) risk at app via to-app from webapp</t>
+  </si>
+  <si>
+    <t>CSRF Prevention</t>
+  </si>
+  <si>
+    <t>Try to use anti-CSRF tokens ot the double-submit patterns (at least for logged-in requests). When your authentication scheme depends on cookies (like session or token cookies), consider marking them with the same-site flag. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>cross-site-request-forgery@app@webapp&gt;to-app</t>
+  </si>
+  <si>
+    <t>Cross-Site Request Forgery (CSRF) risk at webapp via to-webapp from client</t>
+  </si>
+  <si>
+    <t>cross-site-request-forgery@webapp@client&gt;to-webapp</t>
+  </si>
+  <si>
+    <t>CWE-1127</t>
+  </si>
+  <si>
+    <t>Missing Build Infrastructure</t>
+  </si>
+  <si>
+    <t>Missing Build Infrastructure in the threat model (referencing asset app as an example)</t>
+  </si>
+  <si>
+    <t>Build Pipeline Hardening</t>
+  </si>
+  <si>
+    <t>Include the build infrastructure in the model.</t>
+  </si>
+  <si>
+    <t>missing-build-infrastructure@app</t>
+  </si>
+  <si>
+    <t>CWE-16</t>
+  </si>
+  <si>
+    <t>Missing Hardening</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at database</t>
+  </si>
+  <si>
+    <t>System Hardening</t>
+  </si>
+  <si>
+    <t>Try to apply all hardening best practices (like CIS benchmarks, OWASP recommendations, vendor recommendations, DevSec Hardening Framework, DBSAT for Oracle databases, and others).</t>
+  </si>
+  <si>
+    <t>missing-hardening@database</t>
   </si>
   <si>
     <t>Business Side</t>
   </si>
   <si>
-    <t>CWE-693</t>
-  </si>
-  <si>
-    <t>Some Individual Risk Example</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Example Individual Risk at Some Technical Asset</t>
-  </si>
-  <si>
-    <t>Some text describing the action...</t>
-  </si>
-  <si>
-    <t>Some text describing the mitigation...</t>
-  </si>
-  <si>
-    <t>Check if XYZ...</t>
-  </si>
-  <si>
-    <t>something-strange@some-component</t>
-  </si>
-  <si>
-    <t>Unchecked</t>
-  </si>
-  <si>
-    <t>Elevated</t>
-  </si>
-  <si>
-    <t>Elevation of Privilege</t>
-  </si>
-  <si>
-    <t>Architecture</t>
-  </si>
-  <si>
-    <t>CWE-306</t>
-  </si>
-  <si>
-    <t>Missing Authentication</t>
-  </si>
-  <si>
-    <t>Server</t>
-  </si>
-  <si>
-    <t>Some Traffic</t>
-  </si>
-  <si>
-    <t>Missing Authentication covering communication link Some Traffic from Client2 to Server</t>
-  </si>
-  <si>
-    <t>Authentication of Incoming Requests</t>
-  </si>
-  <si>
-    <t>Apply an authentication method to the technical asset. To protect highly sensitive data consider the use of two-factor authentication for human users.</t>
-  </si>
-  <si>
-    <t>Are recommendations from the linked cheat sheet and referenced ASVS chapter applied?</t>
-  </si>
-  <si>
-    <t>missing-authentication@some-component2&gt;some-traffic@some-component2@some-other-component</t>
-  </si>
-  <si>
-    <t>Missing Authentication covering communication link Some Traffic from Client to Server</t>
-  </si>
-  <si>
-    <t>missing-authentication@some-component&gt;some-traffic@some-component@some-other-component</t>
-  </si>
-  <si>
-    <t>Very Likely</t>
-  </si>
-  <si>
-    <t>Information Disclosure</t>
-  </si>
-  <si>
-    <t>Development</t>
-  </si>
-  <si>
-    <t>CWE-611</t>
-  </si>
-  <si>
-    <t>XML External Entity (XXE)</t>
-  </si>
-  <si>
-    <t>Client2</t>
-  </si>
-  <si>
-    <t>XML External Entity (XXE) risk at Client2</t>
-  </si>
-  <si>
-    <t>XML Parser Hardening</t>
-  </si>
-  <si>
-    <t>Apply hardening of all XML parser instances in order to stay safe from XML External Entity (XXE) vulnerabilities. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
-  </si>
-  <si>
-    <t>xml-external-entity@some-component2</t>
-  </si>
-  <si>
-    <t>XML External Entity (XXE) risk at Client</t>
-  </si>
-  <si>
-    <t>xml-external-entity@some-component</t>
-  </si>
-  <si>
-    <t>XML External Entity (XXE) risk at Server</t>
-  </si>
-  <si>
-    <t>xml-external-entity@some-other-component</t>
-  </si>
-  <si>
-    <t>Unlikely</t>
-  </si>
-  <si>
-    <t>Tampering</t>
-  </si>
-  <si>
-    <t>CWE-1127</t>
-  </si>
-  <si>
-    <t>Missing Build Infrastructure</t>
-  </si>
-  <si>
-    <t>Missing Build Infrastructure in the threat model (referencing asset Client as an example)</t>
-  </si>
-  <si>
-    <t>Build Pipeline Hardening</t>
-  </si>
-  <si>
-    <t>Include the build infrastructure in the model.</t>
-  </si>
-  <si>
-    <t>missing-build-infrastructure@some-component</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Operations</t>
-  </si>
-  <si>
-    <t>CWE-16</t>
-  </si>
-  <si>
-    <t>Missing Hardening</t>
-  </si>
-  <si>
-    <t>Missing Hardening risk at Client2</t>
-  </si>
-  <si>
-    <t>System Hardening</t>
-  </si>
-  <si>
-    <t>Try to apply all hardening best practices (like CIS benchmarks, OWASP recommendations, vendor recommendations, DevSec Hardening Framework, DBSAT for Oracle databases, and others).</t>
-  </si>
-  <si>
-    <t>missing-hardening@some-component2</t>
-  </si>
-  <si>
-    <t>Missing Hardening risk at Client</t>
-  </si>
-  <si>
-    <t>missing-hardening@some-component</t>
-  </si>
-  <si>
     <t>CWE-308</t>
   </si>
   <si>
     <t>Missing Two-Factor Authentication (2FA)</t>
   </si>
   <si>
-    <t>Missing Two-Factor Authentication covering communication link Some Traffic from Client2 to Server</t>
+    <t>Missing Two-Factor Authentication covering communication link to-webapp from client to webapp</t>
   </si>
   <si>
     <t>Authentication with Second Factor (2FA)</t>
@@ -274,13 +325,7 @@
     <t>Apply an authentication method to the technical asset protecting highly sensitive data via two-factor authentication for human users.</t>
   </si>
   <si>
-    <t>missing-authentication-second-factor@some-component2&gt;some-traffic@some-component2@some-other-component</t>
-  </si>
-  <si>
-    <t>Missing Two-Factor Authentication covering communication link Some Traffic from Client to Server</t>
-  </si>
-  <si>
-    <t>missing-authentication-second-factor@some-component&gt;some-traffic@some-component@some-other-component</t>
+    <t>missing-authentication-second-factor@client&gt;to-webapp@client@webapp</t>
   </si>
   <si>
     <t>CWE-522</t>
@@ -289,7 +334,7 @@
     <t>Missing Vault (Secret Storage)</t>
   </si>
   <si>
-    <t>Missing Vault (Secret Storage) in the threat model (referencing asset Client as an example)</t>
+    <t>Missing Vault (Secret Storage) in the threat model (referencing asset app as an example)</t>
   </si>
   <si>
     <t>Vault (Secret Storage)</t>
@@ -301,7 +346,7 @@
     <t>Is a Vault (Secret Storage) in place?</t>
   </si>
   <si>
-    <t>missing-vault@some-component</t>
+    <t>missing-vault@app</t>
   </si>
   <si>
     <t>CWE-918</t>
@@ -310,7 +355,7 @@
     <t>Server-Side Request Forgery (SSRF)</t>
   </si>
   <si>
-    <t>Server-Side Request Forgery (SSRF) risk at Client2 server-side web-requesting the target Server via Some Traffic</t>
+    <t>Server-Side Request Forgery (SSRF) risk at webapp server-side web-requesting the target app via to-app</t>
   </si>
   <si>
     <t>SSRF Prevention</t>
@@ -319,13 +364,7 @@
     <t>Try to avoid constructing the outgoing target URL with caller controllable values. Alternatively use a mapping (whitelist) when accessing outgoing URLs instead of creating them including caller controllable values. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
   </si>
   <si>
-    <t>server-side-request-forgery@some-component2@some-other-component@some-component2&gt;some-traffic</t>
-  </si>
-  <si>
-    <t>Server-Side Request Forgery (SSRF) risk at Client server-side web-requesting the target Server via Some Traffic</t>
-  </si>
-  <si>
-    <t>server-side-request-forgery@some-component@some-other-component@some-component&gt;some-traffic</t>
+    <t>server-side-request-forgery@webapp@app@webapp&gt;to-app</t>
   </si>
   <si>
     <t>CWE-311</t>
@@ -334,7 +373,7 @@
     <t>Unencrypted Technical Assets</t>
   </si>
   <si>
-    <t>Unencrypted Technical Asset named Client2</t>
+    <t>Unencrypted Technical Asset named app</t>
   </si>
   <si>
     <t>Encryption of Technical Asset</t>
@@ -343,61 +382,43 @@
     <t>Apply encryption to the technical asset.</t>
   </si>
   <si>
-    <t>unencrypted-asset@some-component2</t>
-  </si>
-  <si>
-    <t>Unencrypted Technical Asset named Server</t>
-  </si>
-  <si>
-    <t>unencrypted-asset@some-other-component</t>
-  </si>
-  <si>
-    <t>Unencrypted Technical Asset named Client</t>
-  </si>
-  <si>
-    <t>unencrypted-asset@some-component</t>
-  </si>
-  <si>
-    <t>Accepted</t>
-  </si>
-  <si>
-    <t>Risk accepted as tolerable</t>
-  </si>
-  <si>
-    <t>2020-01-04</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>XYZ-1234</t>
-  </si>
-  <si>
-    <t>Denial of Service</t>
-  </si>
-  <si>
-    <t>CWE-400</t>
-  </si>
-  <si>
-    <t>DoS-risky Access Across Trust-Boundary</t>
-  </si>
-  <si>
-    <t>Denial-of-Service risky access of Server by Client2 via Some Traffic</t>
-  </si>
-  <si>
-    <t>Anti-DoS Measures</t>
-  </si>
-  <si>
-    <t>Apply anti-DoS techniques like throttling and/or per-client load blocking with quotas. Also for maintenance access routes consider applying a VPN instead of public reachable interfaces. Generally applying redundancy on the targeted technical asset reduces the risk of DoS.</t>
-  </si>
-  <si>
-    <t>dos-risky-access-across-trust-boundary@some-other-component@some-component2@some-component2&gt;some-traffic</t>
-  </si>
-  <si>
-    <t>Denial-of-Service risky access of Server by Client via Some Traffic</t>
-  </si>
-  <si>
-    <t>dos-risky-access-across-trust-boundary@some-other-component@some-component@some-component&gt;some-traffic</t>
+    <t>unencrypted-asset@app</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named client</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@client</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named database</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@database</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named webapp</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@webapp</t>
+  </si>
+  <si>
+    <t>CWE-501</t>
+  </si>
+  <si>
+    <t>Unguarded Access From Internet</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of app by webapp via to-app</t>
+  </si>
+  <si>
+    <t>Encapsulation of Technical Asset</t>
+  </si>
+  <si>
+    <t>Encapsulate the asset behind a guarding service, application, or reverse-proxy. For admin maintenance a bastion-host should be used as a jump-server. For file transfer a store-and-forward-host should be used as an indirect file exchange platform.</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@app@webapp@webapp&gt;to-app</t>
   </si>
   <si>
     <t>CWE-1008</t>
@@ -406,7 +427,7 @@
     <t>Missing Network Segmentation</t>
   </si>
   <si>
-    <t>Missing Network Segmentation to further encapsulate and protect Client2 against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+    <t>Missing Network Segmentation to further encapsulate and protect database against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
   </si>
   <si>
     <t>Network Segmentation</t>
@@ -415,19 +436,13 @@
     <t>Apply a network segmentation trust-boundary around the highly sensitive assets and/or datastores.</t>
   </si>
   <si>
-    <t>missing-network-segmentation@some-component2</t>
-  </si>
-  <si>
-    <t>Missing Network Segmentation to further encapsulate and protect Client against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
-  </si>
-  <si>
-    <t>missing-network-segmentation@some-component</t>
+    <t>missing-network-segmentation@database</t>
   </si>
   <si>
     <t>Missing Web Application Firewall (WAF)</t>
   </si>
   <si>
-    <t>Missing Web Application Firewall (WAF) risk at Server</t>
+    <t>Missing Web Application Firewall (WAF) risk at app</t>
   </si>
   <si>
     <t>Web Application Firewall (WAF)</t>
@@ -439,22 +454,13 @@
     <t>Is a Web Application Firewall (WAF) in place?</t>
   </si>
   <si>
-    <t>missing-waf@some-other-component</t>
-  </si>
-  <si>
-    <t>Mixed Targets on Shared Runtime</t>
-  </si>
-  <si>
-    <t>Mixed Targets on Shared Runtime named Some Shared Runtime might enable attackers moving from one less valuable target to a more valuable one</t>
-  </si>
-  <si>
-    <t>Runtime Separation</t>
-  </si>
-  <si>
-    <t>Use separate runtime environments for running different target components or apply similar separation styles to prevent load- or breach-related problems originating from one more attacker-facing asset impacts also the other more critical rated backend/datastore assets.</t>
-  </si>
-  <si>
-    <t>mixed-targets-on-shared-runtime@some-runtime</t>
+    <t>missing-waf@app</t>
+  </si>
+  <si>
+    <t>Missing Web Application Firewall (WAF) risk at webapp</t>
+  </si>
+  <si>
+    <t>missing-waf@webapp</t>
   </si>
 </sst>
 </file>
@@ -1051,35 +1057,35 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J2" s="18">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>29</v>
@@ -1106,7 +1112,7 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>21</v>
@@ -1115,40 +1121,40 @@
         <v>22</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J3" s="18">
         <v>1</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L3" s="22" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="N3" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>34</v>
@@ -1160,7 +1166,7 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>21</v>
@@ -1169,40 +1175,40 @@
         <v>22</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J4" s="18">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>34</v>
@@ -1214,49 +1220,49 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J5" s="18">
         <v>100</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P5" s="10" t="s">
         <v>34</v>
@@ -1268,49 +1274,49 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="J6" s="18">
+        <v>1</v>
+      </c>
+      <c r="K6" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="L6" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="18">
-        <v>100</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>60</v>
       </c>
       <c r="P6" s="10" t="s">
         <v>34</v>
@@ -1322,49 +1328,49 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J7" s="18">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>34</v>
@@ -1375,50 +1381,50 @@
       <c r="T7" s="16"/>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="H8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="18">
+        <v>1</v>
+      </c>
+      <c r="K8" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="L8" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="18">
-        <v>100</v>
-      </c>
-      <c r="K8" s="19" t="s">
+      <c r="M8" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="N8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="N8" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>70</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>34</v>
@@ -1429,50 +1435,50 @@
       <c r="T8" s="16"/>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="18">
+        <v>1</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="18">
-        <v>100</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="M9" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="N9" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="20" t="s">
-        <v>78</v>
       </c>
       <c r="P9" s="10" t="s">
         <v>34</v>
@@ -1487,46 +1493,46 @@
         <v>22</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="J10" s="18">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O10" s="20" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="P10" s="10" t="s">
         <v>34</v>
@@ -1541,46 +1547,46 @@
         <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="18">
+        <v>30</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="M11" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="N11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="20" t="s">
         <v>82</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="18">
-        <v>1</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="L11" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="M11" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="N11" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>86</v>
       </c>
       <c r="P11" s="10" t="s">
         <v>34</v>
@@ -1595,46 +1601,46 @@
         <v>22</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="J12" s="18">
         <v>1</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="20" t="s">
         <v>84</v>
-      </c>
-      <c r="M12" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="N12" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O12" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="P12" s="10" t="s">
         <v>34</v>
@@ -1649,22 +1655,22 @@
         <v>22</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>27</v>
@@ -1673,22 +1679,22 @@
         <v>28</v>
       </c>
       <c r="J13" s="18">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="O13" s="20" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="P13" s="10" t="s">
         <v>34</v>
@@ -1706,43 +1712,43 @@
         <v>21</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J14" s="18">
         <v>100</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N14" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O14" s="20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="P14" s="10" t="s">
         <v>34</v>
@@ -1757,43 +1763,43 @@
         <v>22</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="J15" s="18">
+        <v>1</v>
+      </c>
+      <c r="K15" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="L15" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="M15" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="L15" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="M15" s="22" t="s">
-        <v>100</v>
-      </c>
       <c r="N15" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O15" s="20" t="s">
         <v>103</v>
@@ -1811,16 +1817,16 @@
         <v>22</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>104</v>
@@ -1829,13 +1835,13 @@
         <v>105</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J16" s="18">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K16" s="19" t="s">
         <v>106</v>
@@ -1847,10 +1853,10 @@
         <v>108</v>
       </c>
       <c r="N16" s="22" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="O16" s="20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="P16" s="10" t="s">
         <v>34</v>
@@ -1865,46 +1871,46 @@
         <v>22</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="J17" s="18">
         <v>1</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O17" s="20" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="P17" s="10" t="s">
         <v>34</v>
@@ -1919,22 +1925,22 @@
         <v>22</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>27</v>
@@ -1943,84 +1949,76 @@
         <v>28</v>
       </c>
       <c r="J18" s="18">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="N18" s="22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O18" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="P18" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q18" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="R18" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="S18" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="16"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="T18" s="16" t="s">
+      <c r="G19" s="7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>41</v>
+      <c r="H19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="J19" s="18">
         <v>1</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M19" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19" s="20" t="s">
         <v>124</v>
-      </c>
-      <c r="N19" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O19" s="20" t="s">
-        <v>125</v>
       </c>
       <c r="P19" s="10" t="s">
         <v>34</v>
@@ -2031,50 +2029,50 @@
       <c r="T19" s="16"/>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="10" t="s">
+      <c r="A20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="C20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="18">
+        <v>100</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="L20" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="M20" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20" s="18">
-        <v>1</v>
-      </c>
-      <c r="K20" s="19" t="s">
+      <c r="N20" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O20" s="20" t="s">
         <v>126</v>
-      </c>
-      <c r="L20" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="M20" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="N20" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" s="20" t="s">
-        <v>127</v>
       </c>
       <c r="P20" s="10" t="s">
         <v>34</v>
@@ -2085,50 +2083,50 @@
       <c r="T20" s="16"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="10" t="s">
+      <c r="A21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="C21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="18">
+        <v>1</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="M21" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="N21" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O21" s="20" t="s">
         <v>128</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="18">
-        <v>100</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="L21" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="M21" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="N21" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O21" s="20" t="s">
-        <v>133</v>
       </c>
       <c r="P21" s="10" t="s">
         <v>34</v>
@@ -2139,50 +2137,50 @@
       <c r="T21" s="16"/>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="G22" s="9" t="s">
+      <c r="A22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="G22" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>28</v>
+      <c r="I22" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="J22" s="18">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K22" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="M22" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="N22" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" s="20" t="s">
         <v>134</v>
-      </c>
-      <c r="L22" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="M22" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="N22" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="O22" s="20" t="s">
-        <v>135</v>
       </c>
       <c r="P22" s="10" t="s">
         <v>34</v>
@@ -2194,34 +2192,34 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>136</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J23" s="18">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K23" s="19" t="s">
         <v>137</v>
@@ -2233,10 +2231,10 @@
         <v>139</v>
       </c>
       <c r="N23" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" s="20" t="s">
         <v>140</v>
-      </c>
-      <c r="O23" s="20" t="s">
-        <v>141</v>
       </c>
       <c r="P23" s="10" t="s">
         <v>34</v>
@@ -2248,46 +2246,46 @@
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J24" s="18">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K24" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="L24" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="M24" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="N24" s="22" t="s">
         <v>145</v>
-      </c>
-      <c r="N24" s="22" t="s">
-        <v>45</v>
       </c>
       <c r="O24" s="20" t="s">
         <v>146</v>
@@ -2299,6 +2297,60 @@
       <c r="R24" s="17"/>
       <c r="S24" s="17"/>
       <c r="T24" s="16"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="18">
+        <v>1</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="M25" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="O25" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="16"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>
@@ -2307,7 +2359,7 @@
     <oddFooter>&amp;C&amp;F</oddFooter>
     <evenHeader>&amp;L&amp;P</evenHeader>
     <evenFooter>&amp;L&amp;D&amp;R&amp;T</evenFooter>
-    <firstHeader>&amp;Threat Model &amp;"-,Wahlpflichtmodul"Bold&amp;"-,Regular"Risks Summary+000A&amp;D</firstHeader>
+    <firstHeader>&amp;Threat Model &amp;"-,Insecure IT Testmodell"Bold&amp;"-,Regular"Risks Summary+000A&amp;D</firstHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>